<commit_message>
added fis sdu report
</commit_message>
<xml_diff>
--- a/survey/dq/dif - check.xlsx
+++ b/survey/dq/dif - check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hb-fidy\Desktop\Python\survey_proj\survey\dq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E00BACF-5B1C-402E-861B-B23982100643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C31D50-8ACC-406E-9D31-CF6A5E55405E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="315" windowWidth="17535" windowHeight="13545" activeTab="1" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
   </bookViews>
   <sheets>
     <sheet name="PR-IFH" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
   <si>
     <t>FH</t>
   </si>
@@ -166,6 +166,39 @@
   </si>
   <si>
     <t>NOK</t>
+  </si>
+  <si>
+    <t>13/jun</t>
+  </si>
+  <si>
+    <t>ME- FH01</t>
+  </si>
+  <si>
+    <t>ME-FH02</t>
+  </si>
+  <si>
+    <t>A1-Roeselare</t>
+  </si>
+  <si>
+    <t>A1-Knokke-Heist</t>
+  </si>
+  <si>
+    <t>A2-Hasselt</t>
+  </si>
+  <si>
+    <t>A2-Antwerpen-West</t>
+  </si>
+  <si>
+    <t>SN-FH01</t>
+  </si>
+  <si>
+    <t>SN-FH02</t>
+  </si>
+  <si>
+    <t>A2-Mechelen</t>
+  </si>
+  <si>
+    <t>A2-Sint-Niklaas</t>
   </si>
 </sst>
 </file>
@@ -173,9 +206,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +237,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +318,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -285,10 +355,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -317,23 +387,35 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,7 +429,7 @@
       <numFmt numFmtId="21" formatCode="d/mmm"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="21" formatCode="d/mmm"/>
     </dxf>
     <dxf>
       <font>
@@ -364,7 +446,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="d/mmm"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -383,24 +465,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:E29" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B3:E29" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:F31" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B3:F31" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8A784E96-2008-40A2-9406-458D39647D96}" name="City"/>
     <tableColumn id="2" xr3:uid="{63957BC9-A292-4B81-A171-FAE41DDDA02E}" name="FH"/>
     <tableColumn id="3" xr3:uid="{237612D4-AAAA-45BA-B7BB-A86439969FB0}" name="Check"/>
     <tableColumn id="4" xr3:uid="{575CFA85-2A34-467B-9198-22906C3ED52A}" name="6/jul"/>
+    <tableColumn id="5" xr3:uid="{F5D8500A-B0DE-4C0D-8D89-E8DB9A579E0F}" name="13/jun"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:R7" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B4:R7" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:V10" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B4:V10" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
+  <tableColumns count="21">
     <tableColumn id="14" xr3:uid="{09A3CB08-CC21-4639-9FAF-CEF1EF053B64}" name="Case #LU" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{8F5AA270-73B2-4A23-BD02-F6F019FEDA66}" name="Date" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{8F5AA270-73B2-4A23-BD02-F6F019FEDA66}" name="Date" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{F217A583-098C-462F-87DD-218845A28EBD}" name="Ro-FH01" dataDxfId="1"/>
     <tableColumn id="19" xr3:uid="{C4A41442-6478-47DE-B654-B9979C2D7F71}" name="Ro-FH03" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{25CF3509-EEE2-4362-9932-BD08B5FAE0AE}" name="Ro-FH04"/>
@@ -416,6 +499,10 @@
     <tableColumn id="11" xr3:uid="{60997CFF-753C-48B3-AC2A-883691107760}" name="KH-FH01"/>
     <tableColumn id="12" xr3:uid="{A6067E7D-58E4-4D71-B59D-041095FBA227}" name="KH-FH09"/>
     <tableColumn id="13" xr3:uid="{D15A5F29-E18D-4705-85D4-2273E822C43F}" name="KH-FH011"/>
+    <tableColumn id="15" xr3:uid="{B4ED75FA-C6A5-4B8F-934C-BFC37C9EBC47}" name="ME- FH01"/>
+    <tableColumn id="16" xr3:uid="{A07AE853-BC36-4EE3-8510-D2B573AA292A}" name="ME-FH02"/>
+    <tableColumn id="20" xr3:uid="{B2DA22DC-D0AF-442C-9922-3D080B05A276}" name="SN-FH01"/>
+    <tableColumn id="21" xr3:uid="{8CE3031B-EC24-4D26-8E2C-382D37B428B2}" name="SN-FH02"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -718,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E0832-9D36-4BE1-92B7-A271D7863A68}">
-  <dimension ref="B3:E29"/>
+  <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,9 +817,10 @@
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -745,8 +833,11 @@
       <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -754,8 +845,9 @@
         <v>2</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -763,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -776,8 +868,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -790,8 +885,11 @@
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -804,8 +902,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -816,7 +917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -829,8 +930,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -843,24 +947,33 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -871,7 +984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -879,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -892,8 +1005,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -906,135 +1022,156 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>17</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1042,21 +1179,55 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E29">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>0</v>
       </c>
     </row>
@@ -1071,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A027803-21AE-40AE-BF1E-F656E364081A}">
-  <dimension ref="B2:R7"/>
+  <dimension ref="B2:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,57 +1254,73 @@
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.42578125" customWidth="1"/>
     <col min="6" max="18" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D2" s="14" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-    </row>
-    <row r="3" spans="2:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-    </row>
-    <row r="4" spans="2:18" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="19"/>
+      <c r="N2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="22"/>
+      <c r="P2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="15"/>
+      <c r="U2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="16"/>
+    </row>
+    <row r="3" spans="2:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+    </row>
+    <row r="4" spans="2:22" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>39</v>
       </c>
@@ -1185,18 +1372,27 @@
       <c r="R4" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="1">
-        <v>44080</v>
+        <v>44018</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5">
-        <v>5</v>
-      </c>
       <c r="G5">
         <v>144</v>
       </c>
@@ -1212,12 +1408,6 @@
       <c r="K5">
         <v>213</v>
       </c>
-      <c r="L5">
-        <v>213</v>
-      </c>
-      <c r="M5">
-        <v>368</v>
-      </c>
       <c r="N5">
         <v>243</v>
       </c>
@@ -1228,17 +1418,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="1">
-        <v>44080</v>
+        <v>44018</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6">
-        <v>1048</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -1254,12 +1441,6 @@
       <c r="K6">
         <v>2</v>
       </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>272</v>
       </c>
@@ -1270,17 +1451,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="1">
-        <v>44080</v>
+        <v>44018</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7">
-        <v>2</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -1296,12 +1474,6 @@
       <c r="K7">
         <v>5</v>
       </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
       <c r="N7">
         <v>0</v>
       </c>
@@ -1312,14 +1484,145 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44025</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="N8">
+        <v>125</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="S8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44025</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>18</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>85</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44025</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>39</v>
+      </c>
+      <c r="P10">
+        <v>21</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="S2:T3"/>
+    <mergeCell ref="U2:V3"/>
     <mergeCell ref="G2:H3"/>
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:M3"/>
     <mergeCell ref="P2:R3"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="N2:O3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dq all cluster empty fix in bg
</commit_message>
<xml_diff>
--- a/survey/dq/dif - check.xlsx
+++ b/survey/dq/dif - check.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hb-fidy\Desktop\Python\survey_proj\survey\dq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C31D50-8ACC-406E-9D31-CF6A5E55405E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCAD260-E733-414C-9654-800F9EA8BE0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
+    <workbookView xWindow="7845" yWindow="2310" windowWidth="15360" windowHeight="11505" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
   </bookViews>
   <sheets>
     <sheet name="PR-IFH" sheetId="2" r:id="rId1"/>
-    <sheet name="Frost Progress" sheetId="4" r:id="rId2"/>
+    <sheet name="TSA" sheetId="5" r:id="rId2"/>
+    <sheet name="Frost Progress" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="59">
   <si>
     <t>FH</t>
   </si>
@@ -199,6 +200,18 @@
   </si>
   <si>
     <t>A2-Sint-Niklaas</t>
+  </si>
+  <si>
+    <t>3/aug</t>
+  </si>
+  <si>
+    <t>10/aug</t>
+  </si>
+  <si>
+    <t>11/aug</t>
+  </si>
+  <si>
+    <t>18/aug</t>
   </si>
 </sst>
 </file>
@@ -208,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +263,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF252423"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF252423"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF484644"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF252423"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +386,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -352,10 +401,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -393,6 +443,49 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,17 +504,12 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Ongeldig" xfId="1" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="21" formatCode="d/mmm"/>
     </dxf>
@@ -451,6 +539,9 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -465,22 +556,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:F31" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B3:F31" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:I31" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:I31" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8A784E96-2008-40A2-9406-458D39647D96}" name="City"/>
     <tableColumn id="2" xr3:uid="{63957BC9-A292-4B81-A171-FAE41DDDA02E}" name="FH"/>
     <tableColumn id="3" xr3:uid="{237612D4-AAAA-45BA-B7BB-A86439969FB0}" name="Check"/>
     <tableColumn id="4" xr3:uid="{575CFA85-2A34-467B-9198-22906C3ED52A}" name="6/jul"/>
     <tableColumn id="5" xr3:uid="{F5D8500A-B0DE-4C0D-8D89-E8DB9A579E0F}" name="13/jun"/>
+    <tableColumn id="6" xr3:uid="{6B3FF845-FE7E-419D-BEC1-C75975371735}" name="3/aug"/>
+    <tableColumn id="7" xr3:uid="{B111E48F-87EC-4488-91CD-F4709D612F1F}" name="10/aug"/>
+    <tableColumn id="8" xr3:uid="{97BF8997-A4D1-4D18-B4C4-F9E69138FD4D}" name="18/aug"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:V10" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B4:V10" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EE7B19D-AD26-4623-8619-C1E316A56D54}" name="Tabel22" displayName="Tabel22" ref="B3:H31" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B3:H31" xr:uid="{AE9CD322-81BE-4683-8B51-33FBF2A6F296}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C02A4E8F-1900-4CA2-A7FE-11E355F124A4}" name="City"/>
+    <tableColumn id="2" xr3:uid="{4F788590-2D50-4BA1-B75D-8660E58E2157}" name="FH"/>
+    <tableColumn id="3" xr3:uid="{38799F48-3B02-4755-94C4-8B573A7DC28B}" name="Check"/>
+    <tableColumn id="4" xr3:uid="{35C0B576-6811-4F37-A66C-5876CC574675}" name="6/jul"/>
+    <tableColumn id="5" xr3:uid="{D15CCAAC-2B9D-4E4D-BFC4-A4A22202F3B7}" name="13/jun"/>
+    <tableColumn id="6" xr3:uid="{6C0B1665-B2A7-4947-B9CF-21B31CC7BA5D}" name="3/aug"/>
+    <tableColumn id="7" xr3:uid="{8A5E13C4-0A45-46DC-83DB-6C66495CBB7D}" name="11/aug"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:V16" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B4:V16" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
   <tableColumns count="21">
     <tableColumn id="14" xr3:uid="{09A3CB08-CC21-4639-9FAF-CEF1EF053B64}" name="Case #LU" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{8F5AA270-73B2-4A23-BD02-F6F019FEDA66}" name="Date" dataDxfId="2"/>
@@ -805,13 +915,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E0832-9D36-4BE1-92B7-A271D7863A68}">
-  <dimension ref="B3:F31"/>
+  <dimension ref="B3:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -820,7 +930,7 @@
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="24.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -836,8 +946,17 @@
       <c r="F3" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -847,7 +966,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -855,7 +974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -871,8 +990,14 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -888,8 +1013,14 @@
       <c r="F7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -905,8 +1036,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -916,8 +1050,14 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -933,8 +1073,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -950,8 +1093,14 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -961,8 +1110,14 @@
       <c r="F12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -972,8 +1127,14 @@
       <c r="F13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -984,7 +1145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -992,7 +1153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1008,8 +1169,14 @@
       <c r="F16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1025,8 +1192,17 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1036,16 +1212,34 @@
       <c r="F18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -1058,8 +1252,17 @@
       <c r="F20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1072,8 +1275,17 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1089,8 +1301,14 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -1106,8 +1324,14 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1120,8 +1344,14 @@
       <c r="F24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>22</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -1134,8 +1364,11 @@
       <c r="F25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
       <c r="B26" t="s">
         <v>13</v>
       </c>
@@ -1151,8 +1384,14 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -1168,8 +1407,14 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1185,8 +1430,17 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>35</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -1196,8 +1450,11 @@
       <c r="E29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -1213,8 +1470,14 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -1229,6 +1492,12 @@
       </c>
       <c r="F31">
         <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1241,14 +1510,394 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A027803-21AE-40AE-BF1E-F656E364081A}">
-  <dimension ref="B2:V10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0B4A3F-18DE-4C18-B26A-521E81EF3F87}">
+  <dimension ref="B3:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8">
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A027803-21AE-40AE-BF1E-F656E364081A}">
+  <dimension ref="B2:AC145"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -1260,67 +1909,67 @@
     <col min="22" max="22" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D2" s="21" t="s">
+    <row r="2" spans="2:29">
+      <c r="D2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="22" t="s">
+      <c r="M2" s="34"/>
+      <c r="N2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="29"/>
+      <c r="P2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="15" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="16" t="s">
+      <c r="T2" s="30"/>
+      <c r="U2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="16"/>
-    </row>
-    <row r="3" spans="2:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-    </row>
-    <row r="4" spans="2:22" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="31"/>
+    </row>
+    <row r="3" spans="2:29" ht="26.25" customHeight="1">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+    </row>
+    <row r="4" spans="2:29" s="6" customFormat="1" ht="42.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>39</v>
       </c>
@@ -1385,7 +2034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1418,7 +2067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:29" ht="16.5">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
@@ -1450,8 +2099,10 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AA6" s="15"/>
+      <c r="AC6" s="15"/>
+    </row>
+    <row r="7" spans="2:29" ht="16.5">
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
@@ -1483,8 +2134,10 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AA7" s="17"/>
+      <c r="AC7" s="17"/>
+    </row>
+    <row r="8" spans="2:29" ht="16.5">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
@@ -1526,8 +2179,10 @@
       <c r="S8">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AA8" s="18"/>
+      <c r="AC8" s="18"/>
+    </row>
+    <row r="9" spans="2:29" ht="16.5">
       <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1569,8 +2224,10 @@
       <c r="S9">
         <v>189</v>
       </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AA9" s="18"/>
+      <c r="AC9" s="18"/>
+    </row>
+    <row r="10" spans="2:29" ht="16.5">
       <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1612,6 +2269,722 @@
       <c r="S10">
         <v>6</v>
       </c>
+      <c r="AA10" s="18"/>
+      <c r="AC10" s="18"/>
+    </row>
+    <row r="11" spans="2:29" ht="16.5">
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44047</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="G11">
+        <v>127</v>
+      </c>
+      <c r="K11">
+        <v>49</v>
+      </c>
+      <c r="N11">
+        <v>11</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="17"/>
+      <c r="AC11" s="17"/>
+    </row>
+    <row r="12" spans="2:29" ht="16.5">
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44047</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="G12">
+        <v>93</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="N12">
+        <v>35</v>
+      </c>
+      <c r="Q12">
+        <v>41</v>
+      </c>
+      <c r="AA12" s="18"/>
+      <c r="AC12" s="18"/>
+    </row>
+    <row r="13" spans="2:29" ht="16.5">
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44047</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>35</v>
+      </c>
+      <c r="P13">
+        <v>21</v>
+      </c>
+      <c r="R13">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="19"/>
+      <c r="AC13" s="19"/>
+    </row>
+    <row r="14" spans="2:29">
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44055</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>26</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>34</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>27</v>
+      </c>
+      <c r="S14">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="20"/>
+      <c r="AC14" s="20"/>
+    </row>
+    <row r="15" spans="2:29" ht="23.25">
+      <c r="B15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44055</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>376</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>8</v>
+      </c>
+      <c r="N15">
+        <v>20</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>43</v>
+      </c>
+      <c r="Q15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <v>362</v>
+      </c>
+      <c r="AA15" s="21"/>
+      <c r="AC15" s="21"/>
+    </row>
+    <row r="16" spans="2:29">
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44055</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>35</v>
+      </c>
+      <c r="P16">
+        <v>21</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="16"/>
+      <c r="AC16" s="16"/>
+    </row>
+    <row r="17" spans="27:29" ht="16.5">
+      <c r="AA17" s="17"/>
+      <c r="AC17" s="17"/>
+    </row>
+    <row r="18" spans="27:29" ht="16.5">
+      <c r="AA18" s="22"/>
+      <c r="AC18" s="22"/>
+    </row>
+    <row r="19" spans="27:29" ht="16.5">
+      <c r="AA19" s="23"/>
+      <c r="AC19" s="23"/>
+    </row>
+    <row r="20" spans="27:29" ht="16.5">
+      <c r="AA20" s="22"/>
+      <c r="AC20" s="22"/>
+    </row>
+    <row r="21" spans="27:29" ht="16.5">
+      <c r="AA21" s="17"/>
+      <c r="AC21" s="17"/>
+    </row>
+    <row r="22" spans="27:29" ht="16.5">
+      <c r="AA22" s="24"/>
+      <c r="AC22" s="24"/>
+    </row>
+    <row r="23" spans="27:29" ht="16.5">
+      <c r="AA23" s="23"/>
+      <c r="AC23" s="23"/>
+    </row>
+    <row r="24" spans="27:29" ht="16.5">
+      <c r="AA24" s="24"/>
+      <c r="AC24" s="24"/>
+    </row>
+    <row r="25" spans="27:29" ht="16.5">
+      <c r="AA25" s="25"/>
+      <c r="AC25" s="25"/>
+    </row>
+    <row r="26" spans="27:29" ht="16.5">
+      <c r="AA26" s="24"/>
+      <c r="AC26" s="24"/>
+    </row>
+    <row r="27" spans="27:29" ht="16.5">
+      <c r="AA27" s="23"/>
+      <c r="AC27" s="23"/>
+    </row>
+    <row r="28" spans="27:29" ht="16.5">
+      <c r="AA28" s="24"/>
+      <c r="AC28" s="24"/>
+    </row>
+    <row r="29" spans="27:29" ht="16.5">
+      <c r="AA29" s="25"/>
+      <c r="AC29" s="25"/>
+    </row>
+    <row r="30" spans="27:29" ht="16.5">
+      <c r="AA30" s="24"/>
+      <c r="AC30" s="24"/>
+    </row>
+    <row r="31" spans="27:29" ht="16.5">
+      <c r="AA31" s="23"/>
+      <c r="AC31" s="23"/>
+    </row>
+    <row r="32" spans="27:29" ht="16.5">
+      <c r="AA32" s="24"/>
+      <c r="AC32" s="24"/>
+    </row>
+    <row r="33" spans="27:29" ht="16.5">
+      <c r="AA33" s="25"/>
+      <c r="AC33" s="25"/>
+    </row>
+    <row r="34" spans="27:29" ht="16.5">
+      <c r="AA34" s="24"/>
+      <c r="AC34" s="24"/>
+    </row>
+    <row r="35" spans="27:29" ht="16.5">
+      <c r="AA35" s="26"/>
+      <c r="AC35" s="26"/>
+    </row>
+    <row r="36" spans="27:29" ht="16.5">
+      <c r="AA36" s="24"/>
+      <c r="AC36" s="24"/>
+    </row>
+    <row r="37" spans="27:29" ht="16.5">
+      <c r="AA37" s="25"/>
+      <c r="AC37" s="25"/>
+    </row>
+    <row r="38" spans="27:29" ht="16.5">
+      <c r="AA38" s="24"/>
+      <c r="AC38" s="24"/>
+    </row>
+    <row r="39" spans="27:29" ht="16.5">
+      <c r="AA39" s="26"/>
+      <c r="AC39" s="26"/>
+    </row>
+    <row r="40" spans="27:29" ht="16.5">
+      <c r="AA40" s="24"/>
+      <c r="AC40" s="24"/>
+    </row>
+    <row r="41" spans="27:29" ht="16.5">
+      <c r="AA41" s="25"/>
+      <c r="AC41" s="25"/>
+    </row>
+    <row r="42" spans="27:29" ht="16.5">
+      <c r="AA42" s="24"/>
+      <c r="AC42" s="24"/>
+    </row>
+    <row r="43" spans="27:29" ht="16.5">
+      <c r="AA43" s="26"/>
+      <c r="AC43" s="26"/>
+    </row>
+    <row r="44" spans="27:29" ht="16.5">
+      <c r="AA44" s="24"/>
+      <c r="AC44" s="24"/>
+    </row>
+    <row r="45" spans="27:29" ht="16.5">
+      <c r="AA45" s="25"/>
+      <c r="AC45" s="25"/>
+    </row>
+    <row r="46" spans="27:29" ht="16.5">
+      <c r="AA46" s="24"/>
+      <c r="AC46" s="24"/>
+    </row>
+    <row r="47" spans="27:29" ht="16.5">
+      <c r="AA47" s="26"/>
+      <c r="AC47" s="26"/>
+    </row>
+    <row r="48" spans="27:29" ht="16.5">
+      <c r="AA48" s="24"/>
+      <c r="AC48" s="24"/>
+    </row>
+    <row r="49" spans="27:29" ht="16.5">
+      <c r="AA49" s="25"/>
+      <c r="AC49" s="25"/>
+    </row>
+    <row r="50" spans="27:29" ht="16.5">
+      <c r="AA50" s="24"/>
+      <c r="AC50" s="24"/>
+    </row>
+    <row r="51" spans="27:29" ht="16.5">
+      <c r="AA51" s="26"/>
+      <c r="AC51" s="26"/>
+    </row>
+    <row r="52" spans="27:29" ht="16.5">
+      <c r="AA52" s="24"/>
+      <c r="AC52" s="24"/>
+    </row>
+    <row r="53" spans="27:29" ht="16.5">
+      <c r="AA53" s="25"/>
+      <c r="AC53" s="25"/>
+    </row>
+    <row r="54" spans="27:29" ht="16.5">
+      <c r="AA54" s="24"/>
+      <c r="AC54" s="24"/>
+    </row>
+    <row r="55" spans="27:29" ht="16.5">
+      <c r="AA55" s="26"/>
+      <c r="AC55" s="26"/>
+    </row>
+    <row r="56" spans="27:29" ht="16.5">
+      <c r="AA56" s="24"/>
+      <c r="AC56" s="24"/>
+    </row>
+    <row r="57" spans="27:29" ht="16.5">
+      <c r="AA57" s="25"/>
+      <c r="AC57" s="25"/>
+    </row>
+    <row r="58" spans="27:29" ht="16.5">
+      <c r="AA58" s="24"/>
+      <c r="AC58" s="24"/>
+    </row>
+    <row r="59" spans="27:29" ht="16.5">
+      <c r="AA59" s="26"/>
+      <c r="AC59" s="26"/>
+    </row>
+    <row r="60" spans="27:29" ht="16.5">
+      <c r="AA60" s="24"/>
+      <c r="AC60" s="24"/>
+    </row>
+    <row r="61" spans="27:29" ht="16.5">
+      <c r="AA61" s="25"/>
+      <c r="AC61" s="25"/>
+    </row>
+    <row r="62" spans="27:29" ht="16.5">
+      <c r="AA62" s="24"/>
+      <c r="AC62" s="24"/>
+    </row>
+    <row r="63" spans="27:29" ht="16.5">
+      <c r="AA63" s="26"/>
+      <c r="AC63" s="26"/>
+    </row>
+    <row r="64" spans="27:29" ht="16.5">
+      <c r="AA64" s="24"/>
+      <c r="AC64" s="24"/>
+    </row>
+    <row r="65" spans="27:29" ht="16.5">
+      <c r="AA65" s="25"/>
+      <c r="AC65" s="25"/>
+    </row>
+    <row r="66" spans="27:29" ht="16.5">
+      <c r="AA66" s="24"/>
+      <c r="AC66" s="24"/>
+    </row>
+    <row r="67" spans="27:29" ht="16.5">
+      <c r="AA67" s="26"/>
+      <c r="AC67" s="26"/>
+    </row>
+    <row r="68" spans="27:29" ht="16.5">
+      <c r="AA68" s="24"/>
+      <c r="AC68" s="24"/>
+    </row>
+    <row r="69" spans="27:29" ht="16.5">
+      <c r="AA69" s="25"/>
+      <c r="AC69" s="25"/>
+    </row>
+    <row r="70" spans="27:29" ht="16.5">
+      <c r="AA70" s="24"/>
+      <c r="AC70" s="24"/>
+    </row>
+    <row r="71" spans="27:29" ht="16.5">
+      <c r="AA71" s="26"/>
+      <c r="AC71" s="26"/>
+    </row>
+    <row r="72" spans="27:29" ht="16.5">
+      <c r="AA72" s="24"/>
+      <c r="AC72" s="24"/>
+    </row>
+    <row r="73" spans="27:29" ht="16.5">
+      <c r="AA73" s="25"/>
+      <c r="AC73" s="25"/>
+    </row>
+    <row r="74" spans="27:29" ht="16.5">
+      <c r="AA74" s="24"/>
+      <c r="AC74" s="24"/>
+    </row>
+    <row r="75" spans="27:29" ht="16.5">
+      <c r="AA75" s="26"/>
+      <c r="AC75" s="26"/>
+    </row>
+    <row r="76" spans="27:29" ht="16.5">
+      <c r="AA76" s="24"/>
+      <c r="AC76" s="24"/>
+    </row>
+    <row r="77" spans="27:29" ht="16.5">
+      <c r="AA77" s="25"/>
+      <c r="AC77" s="25"/>
+    </row>
+    <row r="78" spans="27:29" ht="16.5">
+      <c r="AA78" s="24"/>
+      <c r="AC78" s="24"/>
+    </row>
+    <row r="79" spans="27:29" ht="16.5">
+      <c r="AA79" s="26"/>
+      <c r="AC79" s="26"/>
+    </row>
+    <row r="80" spans="27:29" ht="16.5">
+      <c r="AA80" s="24"/>
+      <c r="AC80" s="24"/>
+    </row>
+    <row r="81" spans="27:29" ht="16.5">
+      <c r="AA81" s="25"/>
+      <c r="AC81" s="25"/>
+    </row>
+    <row r="82" spans="27:29" ht="16.5">
+      <c r="AA82" s="24"/>
+      <c r="AC82" s="24"/>
+    </row>
+    <row r="83" spans="27:29" ht="16.5">
+      <c r="AA83" s="26"/>
+      <c r="AC83" s="26"/>
+    </row>
+    <row r="84" spans="27:29" ht="16.5">
+      <c r="AA84" s="24"/>
+      <c r="AC84" s="24"/>
+    </row>
+    <row r="85" spans="27:29" ht="16.5">
+      <c r="AA85" s="25"/>
+      <c r="AC85" s="25"/>
+    </row>
+    <row r="86" spans="27:29" ht="16.5">
+      <c r="AA86" s="24"/>
+      <c r="AC86" s="24"/>
+    </row>
+    <row r="87" spans="27:29" ht="16.5">
+      <c r="AA87" s="26"/>
+      <c r="AC87" s="26"/>
+    </row>
+    <row r="88" spans="27:29" ht="16.5">
+      <c r="AA88" s="24"/>
+      <c r="AC88" s="24"/>
+    </row>
+    <row r="89" spans="27:29" ht="16.5">
+      <c r="AA89" s="25"/>
+      <c r="AC89" s="25"/>
+    </row>
+    <row r="90" spans="27:29" ht="16.5">
+      <c r="AA90" s="24"/>
+      <c r="AC90" s="24"/>
+    </row>
+    <row r="91" spans="27:29" ht="16.5">
+      <c r="AA91" s="26"/>
+      <c r="AC91" s="26"/>
+    </row>
+    <row r="92" spans="27:29" ht="16.5">
+      <c r="AA92" s="24"/>
+      <c r="AC92" s="24"/>
+    </row>
+    <row r="93" spans="27:29" ht="16.5">
+      <c r="AA93" s="25"/>
+      <c r="AC93" s="25"/>
+    </row>
+    <row r="94" spans="27:29" ht="16.5">
+      <c r="AA94" s="24"/>
+      <c r="AC94" s="24"/>
+    </row>
+    <row r="95" spans="27:29" ht="16.5">
+      <c r="AA95" s="26"/>
+      <c r="AC95" s="26"/>
+    </row>
+    <row r="96" spans="27:29" ht="16.5">
+      <c r="AA96" s="24"/>
+      <c r="AC96" s="24"/>
+    </row>
+    <row r="97" spans="27:29" ht="16.5">
+      <c r="AA97" s="25"/>
+      <c r="AC97" s="25"/>
+    </row>
+    <row r="98" spans="27:29" ht="16.5">
+      <c r="AA98" s="24"/>
+      <c r="AC98" s="24"/>
+    </row>
+    <row r="99" spans="27:29" ht="16.5">
+      <c r="AA99" s="26"/>
+      <c r="AC99" s="26"/>
+    </row>
+    <row r="100" spans="27:29" ht="16.5">
+      <c r="AA100" s="24"/>
+      <c r="AC100" s="24"/>
+    </row>
+    <row r="101" spans="27:29" ht="16.5">
+      <c r="AA101" s="25"/>
+      <c r="AC101" s="25"/>
+    </row>
+    <row r="102" spans="27:29" ht="16.5">
+      <c r="AA102" s="24"/>
+      <c r="AC102" s="24"/>
+    </row>
+    <row r="103" spans="27:29" ht="16.5">
+      <c r="AA103" s="26"/>
+      <c r="AC103" s="26"/>
+    </row>
+    <row r="104" spans="27:29" ht="16.5">
+      <c r="AA104" s="24"/>
+      <c r="AC104" s="24"/>
+    </row>
+    <row r="105" spans="27:29" ht="16.5">
+      <c r="AA105" s="25"/>
+      <c r="AC105" s="25"/>
+    </row>
+    <row r="106" spans="27:29" ht="16.5">
+      <c r="AA106" s="24"/>
+      <c r="AC106" s="24"/>
+    </row>
+    <row r="107" spans="27:29" ht="16.5">
+      <c r="AA107" s="26"/>
+      <c r="AC107" s="26"/>
+    </row>
+    <row r="108" spans="27:29" ht="16.5">
+      <c r="AA108" s="24"/>
+      <c r="AC108" s="24"/>
+    </row>
+    <row r="109" spans="27:29" ht="16.5">
+      <c r="AA109" s="25"/>
+      <c r="AC109" s="25"/>
+    </row>
+    <row r="110" spans="27:29" ht="16.5">
+      <c r="AA110" s="24"/>
+      <c r="AC110" s="24"/>
+    </row>
+    <row r="111" spans="27:29" ht="16.5">
+      <c r="AA111" s="26"/>
+      <c r="AC111" s="26"/>
+    </row>
+    <row r="112" spans="27:29" ht="16.5">
+      <c r="AA112" s="24"/>
+      <c r="AC112" s="24"/>
+    </row>
+    <row r="113" spans="27:29" ht="16.5">
+      <c r="AA113" s="25"/>
+      <c r="AC113" s="25"/>
+    </row>
+    <row r="114" spans="27:29" ht="16.5">
+      <c r="AA114" s="24"/>
+      <c r="AC114" s="24"/>
+    </row>
+    <row r="115" spans="27:29" ht="16.5">
+      <c r="AA115" s="26"/>
+      <c r="AC115" s="26"/>
+    </row>
+    <row r="116" spans="27:29" ht="16.5">
+      <c r="AA116" s="24"/>
+      <c r="AC116" s="24"/>
+    </row>
+    <row r="117" spans="27:29" ht="16.5">
+      <c r="AA117" s="25"/>
+      <c r="AC117" s="25"/>
+    </row>
+    <row r="118" spans="27:29" ht="16.5">
+      <c r="AA118" s="24"/>
+      <c r="AC118" s="24"/>
+    </row>
+    <row r="119" spans="27:29" ht="16.5">
+      <c r="AA119" s="26"/>
+      <c r="AC119" s="26"/>
+    </row>
+    <row r="120" spans="27:29" ht="16.5">
+      <c r="AA120" s="24"/>
+      <c r="AC120" s="24"/>
+    </row>
+    <row r="121" spans="27:29" ht="16.5">
+      <c r="AA121" s="25"/>
+      <c r="AC121" s="25"/>
+    </row>
+    <row r="122" spans="27:29" ht="16.5">
+      <c r="AA122" s="24"/>
+      <c r="AC122" s="24"/>
+    </row>
+    <row r="123" spans="27:29" ht="16.5">
+      <c r="AA123" s="26"/>
+      <c r="AC123" s="26"/>
+    </row>
+    <row r="124" spans="27:29" ht="16.5">
+      <c r="AA124" s="24"/>
+      <c r="AC124" s="24"/>
+    </row>
+    <row r="125" spans="27:29" ht="16.5">
+      <c r="AA125" s="25"/>
+      <c r="AC125" s="25"/>
+    </row>
+    <row r="126" spans="27:29" ht="16.5">
+      <c r="AA126" s="24"/>
+      <c r="AC126" s="24"/>
+    </row>
+    <row r="127" spans="27:29" ht="16.5">
+      <c r="AA127" s="26"/>
+      <c r="AC127" s="26"/>
+    </row>
+    <row r="128" spans="27:29" ht="16.5">
+      <c r="AA128" s="24"/>
+      <c r="AC128" s="24"/>
+    </row>
+    <row r="129" spans="27:29" ht="16.5">
+      <c r="AA129" s="25"/>
+      <c r="AC129" s="25"/>
+    </row>
+    <row r="130" spans="27:29" ht="16.5">
+      <c r="AA130" s="24"/>
+      <c r="AC130" s="24"/>
+    </row>
+    <row r="131" spans="27:29" ht="16.5">
+      <c r="AA131" s="26"/>
+      <c r="AC131" s="26"/>
+    </row>
+    <row r="132" spans="27:29" ht="16.5">
+      <c r="AA132" s="24"/>
+      <c r="AC132" s="24"/>
+    </row>
+    <row r="133" spans="27:29" ht="16.5">
+      <c r="AA133" s="25"/>
+      <c r="AC133" s="25"/>
+    </row>
+    <row r="134" spans="27:29" ht="16.5">
+      <c r="AA134" s="24"/>
+      <c r="AC134" s="24"/>
+    </row>
+    <row r="135" spans="27:29" ht="16.5">
+      <c r="AA135" s="26"/>
+      <c r="AC135" s="26"/>
+    </row>
+    <row r="136" spans="27:29" ht="16.5">
+      <c r="AA136" s="24"/>
+      <c r="AC136" s="24"/>
+    </row>
+    <row r="137" spans="27:29" ht="16.5">
+      <c r="AA137" s="25"/>
+      <c r="AC137" s="25"/>
+    </row>
+    <row r="138" spans="27:29" ht="16.5">
+      <c r="AA138" s="24"/>
+      <c r="AC138" s="24"/>
+    </row>
+    <row r="139" spans="27:29" ht="16.5">
+      <c r="AA139" s="26"/>
+      <c r="AC139" s="26"/>
+    </row>
+    <row r="140" spans="27:29" ht="16.5">
+      <c r="AA140" s="24"/>
+      <c r="AC140" s="24"/>
+    </row>
+    <row r="141" spans="27:29" ht="16.5">
+      <c r="AA141" s="25"/>
+      <c r="AC141" s="25"/>
+    </row>
+    <row r="142" spans="27:29" ht="16.5">
+      <c r="AA142" s="24"/>
+      <c r="AC142" s="24"/>
+    </row>
+    <row r="143" spans="27:29" ht="16.5">
+      <c r="AA143" s="26"/>
+      <c r="AC143" s="26"/>
+    </row>
+    <row r="144" spans="27:29" ht="16.5">
+      <c r="AA144" s="24"/>
+      <c r="AC144" s="24"/>
+    </row>
+    <row r="145" spans="27:29" ht="16.5">
+      <c r="AA145" s="25"/>
+      <c r="AC145" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1626,8 +2999,9 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
tsa sharepoint changes + bugfixes
</commit_message>
<xml_diff>
--- a/survey/dq/dif - check.xlsx
+++ b/survey/dq/dif - check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hb-fidy\Desktop\Python\survey_proj\survey\dq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCAD260-E733-414C-9654-800F9EA8BE0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E58CEF-5D48-4D5A-956B-BC3701CD01A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="2310" windowWidth="15360" windowHeight="11505" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E62FDE45-BBFB-4995-BABB-BE1094A9500C}"/>
   </bookViews>
   <sheets>
     <sheet name="PR-IFH" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="66">
   <si>
     <t>FH</t>
   </si>
@@ -212,6 +212,27 @@
   </si>
   <si>
     <t>18/aug</t>
+  </si>
+  <si>
+    <t>24/aug</t>
+  </si>
+  <si>
+    <t>25/aug</t>
+  </si>
+  <si>
+    <t>31/aug</t>
+  </si>
+  <si>
+    <t>7/sep</t>
+  </si>
+  <si>
+    <t>AW-FH06</t>
+  </si>
+  <si>
+    <t>22/sep</t>
+  </si>
+  <si>
+    <t>28/sep</t>
   </si>
 </sst>
 </file>
@@ -483,9 +504,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,6 +521,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -556,9 +577,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:I31" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B3:I31" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D23F1BB3-D746-4908-A60E-81AA4BEADC42}" name="Tabel2" displayName="Tabel2" ref="B3:N31" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:N31" xr:uid="{DB429C94-0748-4920-B073-927B752A3887}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8A784E96-2008-40A2-9406-458D39647D96}" name="City"/>
     <tableColumn id="2" xr3:uid="{63957BC9-A292-4B81-A171-FAE41DDDA02E}" name="FH"/>
     <tableColumn id="3" xr3:uid="{237612D4-AAAA-45BA-B7BB-A86439969FB0}" name="Check"/>
@@ -567,15 +588,20 @@
     <tableColumn id="6" xr3:uid="{6B3FF845-FE7E-419D-BEC1-C75975371735}" name="3/aug"/>
     <tableColumn id="7" xr3:uid="{B111E48F-87EC-4488-91CD-F4709D612F1F}" name="10/aug"/>
     <tableColumn id="8" xr3:uid="{97BF8997-A4D1-4D18-B4C4-F9E69138FD4D}" name="18/aug"/>
+    <tableColumn id="9" xr3:uid="{DA7CEF6F-7A3E-4594-A319-E6D41744A3B1}" name="24/aug"/>
+    <tableColumn id="10" xr3:uid="{B95FE5B2-3D66-4FE3-B180-5BCDBDEFF6FB}" name="31/aug"/>
+    <tableColumn id="11" xr3:uid="{AC75E106-0B13-43E8-8CBE-920E8040FCAE}" name="7/sep"/>
+    <tableColumn id="12" xr3:uid="{495534AD-5BDA-436E-918B-E6A7BFE865F9}" name="22/sep"/>
+    <tableColumn id="13" xr3:uid="{C9A81020-FC22-4844-B5A1-609090D61933}" name="28/sep"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EE7B19D-AD26-4623-8619-C1E316A56D54}" name="Tabel22" displayName="Tabel22" ref="B3:H31" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B3:H31" xr:uid="{AE9CD322-81BE-4683-8B51-33FBF2A6F296}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EE7B19D-AD26-4623-8619-C1E316A56D54}" name="Tabel22" displayName="Tabel22" ref="B3:I31" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B3:I31" xr:uid="{AE9CD322-81BE-4683-8B51-33FBF2A6F296}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C02A4E8F-1900-4CA2-A7FE-11E355F124A4}" name="City"/>
     <tableColumn id="2" xr3:uid="{4F788590-2D50-4BA1-B75D-8660E58E2157}" name="FH"/>
     <tableColumn id="3" xr3:uid="{38799F48-3B02-4755-94C4-8B573A7DC28B}" name="Check"/>
@@ -583,15 +609,16 @@
     <tableColumn id="5" xr3:uid="{D15CCAAC-2B9D-4E4D-BFC4-A4A22202F3B7}" name="13/jun"/>
     <tableColumn id="6" xr3:uid="{6C0B1665-B2A7-4947-B9CF-21B31CC7BA5D}" name="3/aug"/>
     <tableColumn id="7" xr3:uid="{8A5E13C4-0A45-46DC-83DB-6C66495CBB7D}" name="11/aug"/>
+    <tableColumn id="8" xr3:uid="{4E79CF0E-1301-493F-A61A-A1C6015E9231}" name="25/aug"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:V16" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B4:V16" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FA9D9F3-CF5D-44DD-83C8-44F9F6F25A09}" name="Tabel4" displayName="Tabel4" ref="B4:W25" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B4:W25" xr:uid="{AC7D51FD-FAE3-4501-BDA3-7BC34372F48C}"/>
+  <tableColumns count="22">
     <tableColumn id="14" xr3:uid="{09A3CB08-CC21-4639-9FAF-CEF1EF053B64}" name="Case #LU" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{8F5AA270-73B2-4A23-BD02-F6F019FEDA66}" name="Date" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{F217A583-098C-462F-87DD-218845A28EBD}" name="Ro-FH01" dataDxfId="1"/>
@@ -606,6 +633,7 @@
     <tableColumn id="9" xr3:uid="{A4894D9B-2A6D-4228-AC80-34A5CC85D82C}" name="LE-FH03"/>
     <tableColumn id="10" xr3:uid="{39DB8E8A-957A-43ED-B17F-9371543A970F}" name="AW-FH01"/>
     <tableColumn id="18" xr3:uid="{62737F43-8237-42AF-96AE-FAB74C52049E}" name="AW-FH07"/>
+    <tableColumn id="22" xr3:uid="{523ADEFA-C5FA-43DD-AF22-581538EECB66}" name="AW-FH06"/>
     <tableColumn id="11" xr3:uid="{60997CFF-753C-48B3-AC2A-883691107760}" name="KH-FH01"/>
     <tableColumn id="12" xr3:uid="{A6067E7D-58E4-4D71-B59D-041095FBA227}" name="KH-FH09"/>
     <tableColumn id="13" xr3:uid="{D15A5F29-E18D-4705-85D4-2273E822C43F}" name="KH-FH011"/>
@@ -915,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E0832-9D36-4BE1-92B7-A271D7863A68}">
-  <dimension ref="B3:I31"/>
+  <dimension ref="B3:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,7 +958,7 @@
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="24.75" customHeight="1">
+    <row r="3" spans="2:14" ht="24.75" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -955,8 +983,23 @@
       <c r="I3" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -966,7 +1009,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -974,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1019,8 +1062,23 @@
       <c r="I7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1039,8 +1097,17 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1056,8 +1123,23 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:9">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1076,8 +1158,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1099,8 +1184,17 @@
       <c r="I11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -1116,14 +1210,32 @@
       <c r="I12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" t="s">
         <v>23</v>
       </c>
@@ -1133,8 +1245,23 @@
       <c r="I13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1145,7 +1272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:14">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:14">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1175,8 +1302,17 @@
       <c r="I16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1201,8 +1337,17 @@
       <c r="I17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1221,8 +1366,14 @@
       <c r="I18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1238,14 +1389,23 @@
       <c r="I19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
       <c r="E20">
         <v>0</v>
       </c>
@@ -1261,8 +1421,17 @@
       <c r="I20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="J20">
+        <v>31</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1284,8 +1453,14 @@
       <c r="I21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1307,8 +1482,20 @@
       <c r="I22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1517,17 @@
       <c r="I23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1350,8 +1546,17 @@
       <c r="I24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:9">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -1367,8 +1572,17 @@
       <c r="I25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="2:9">
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26" t="s">
         <v>13</v>
       </c>
@@ -1390,8 +1604,17 @@
       <c r="I26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="2:9">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -1413,8 +1636,17 @@
       <c r="I27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="2:9">
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1439,8 +1671,23 @@
       <c r="I28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:9">
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -1453,8 +1700,17 @@
       <c r="I29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="2:9">
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>3</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -1476,8 +1732,20 @@
       <c r="I30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:9">
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -1498,6 +1766,18 @@
       </c>
       <c r="I31">
         <v>1</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1511,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0B4A3F-18DE-4C18-B26A-521E81EF3F87}">
-  <dimension ref="B3:H31"/>
+  <dimension ref="B3:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1522,7 +1802,7 @@
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:9">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1544,8 +1824,11 @@
       <c r="H3" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1555,7 +1838,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1563,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1574,7 +1857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1586,7 +1869,7 @@
       </c>
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1600,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1612,7 +1895,7 @@
       </c>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +1909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1640,7 +1923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -1651,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1673,7 +1956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -1681,7 +1964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1694,8 +1977,11 @@
       <c r="H16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1708,8 +1994,11 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1720,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -1741,8 +2030,11 @@
       <c r="H20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1752,8 +2044,11 @@
       <c r="H21">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1766,8 +2061,11 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -1780,8 +2078,11 @@
       <c r="H23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="I23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1791,8 +2092,11 @@
       <c r="H24">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="I24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -1800,7 +2104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:9">
       <c r="B26" t="s">
         <v>13</v>
       </c>
@@ -1813,8 +2117,11 @@
       <c r="H26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:8">
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -1827,8 +2134,11 @@
       <c r="H27">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="2:8">
+      <c r="I27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1841,8 +2151,11 @@
       <c r="H28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -1853,7 +2166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -1866,8 +2179,11 @@
       <c r="H30">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -1879,6 +2195,9 @@
       </c>
       <c r="H31">
         <v>17</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1891,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A027803-21AE-40AE-BF1E-F656E364081A}">
-  <dimension ref="B2:AC145"/>
+  <dimension ref="B2:AD145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1902,14 +2221,14 @@
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="18" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" customWidth="1"/>
-    <col min="22" max="22" width="7.7109375" customWidth="1"/>
+    <col min="6" max="19" width="7.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:29">
+    <row r="2" spans="2:30" ht="15" customHeight="1">
       <c r="D2" s="28" t="s">
         <v>47</v>
       </c>
@@ -1917,59 +2236,61 @@
       <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34" t="s">
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="35" t="s">
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="30" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="31"/>
-    </row>
-    <row r="3" spans="2:29" ht="26.25" customHeight="1">
+      <c r="W2" s="30"/>
+    </row>
+    <row r="3" spans="2:30" ht="26.25" customHeight="1">
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
       <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-    </row>
-    <row r="4" spans="2:29" s="6" customFormat="1" ht="42.75" customHeight="1">
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+    </row>
+    <row r="4" spans="2:30" s="6" customFormat="1" ht="42.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>39</v>
       </c>
@@ -2012,29 +2333,32 @@
       <c r="O4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="R4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="S4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="U4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="14" t="s">
+      <c r="V4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="W4" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:29">
+    <row r="5" spans="2:30">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -2060,14 +2384,14 @@
       <c r="N5">
         <v>243</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>623</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:29" ht="16.5">
+    <row r="6" spans="2:30" ht="16.5">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
@@ -2093,16 +2417,16 @@
       <c r="N6">
         <v>272</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>100</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="15"/>
-      <c r="AC6" s="15"/>
-    </row>
-    <row r="7" spans="2:29" ht="16.5">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15"/>
+      <c r="AD6" s="15"/>
+    </row>
+    <row r="7" spans="2:30" ht="16.5">
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
@@ -2128,16 +2452,16 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>21</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="17"/>
-      <c r="AC7" s="17"/>
-    </row>
-    <row r="8" spans="2:29" ht="16.5">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="17"/>
+      <c r="AD7" s="17"/>
+    </row>
+    <row r="8" spans="2:30" ht="16.5">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
@@ -2170,19 +2494,19 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>3</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>75</v>
       </c>
-      <c r="AA8" s="18"/>
-      <c r="AC8" s="18"/>
-    </row>
-    <row r="9" spans="2:29" ht="16.5">
+      <c r="AB8" s="18"/>
+      <c r="AD8" s="18"/>
+    </row>
+    <row r="9" spans="2:30" ht="16.5">
       <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
@@ -2215,19 +2539,19 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>2</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>8</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>189</v>
       </c>
-      <c r="AA9" s="18"/>
-      <c r="AC9" s="18"/>
-    </row>
-    <row r="10" spans="2:29" ht="16.5">
+      <c r="AB9" s="18"/>
+      <c r="AD9" s="18"/>
+    </row>
+    <row r="10" spans="2:30" ht="16.5">
       <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
@@ -2260,19 +2584,19 @@
       <c r="O10">
         <v>39</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>21</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="S10">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>6</v>
       </c>
-      <c r="AA10" s="18"/>
-      <c r="AC10" s="18"/>
-    </row>
-    <row r="11" spans="2:29" ht="16.5">
+      <c r="AB10" s="18"/>
+      <c r="AD10" s="18"/>
+    </row>
+    <row r="11" spans="2:30" ht="16.5">
       <c r="B11" s="5" t="s">
         <v>36</v>
       </c>
@@ -2290,16 +2614,16 @@
       <c r="N11">
         <v>11</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>2</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="AA11" s="17"/>
-      <c r="AC11" s="17"/>
-    </row>
-    <row r="12" spans="2:29" ht="16.5">
+      <c r="AB11" s="17"/>
+      <c r="AD11" s="17"/>
+    </row>
+    <row r="12" spans="2:30" ht="16.5">
       <c r="B12" s="5" t="s">
         <v>37</v>
       </c>
@@ -2317,13 +2641,13 @@
       <c r="N12">
         <v>35</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>41</v>
       </c>
-      <c r="AA12" s="18"/>
-      <c r="AC12" s="18"/>
-    </row>
-    <row r="13" spans="2:29" ht="16.5">
+      <c r="AB12" s="18"/>
+      <c r="AD12" s="18"/>
+    </row>
+    <row r="13" spans="2:30" ht="16.5">
       <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
@@ -2344,16 +2668,16 @@
       <c r="O13">
         <v>35</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>21</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>13</v>
       </c>
-      <c r="AA13" s="19"/>
-      <c r="AC13" s="19"/>
-    </row>
-    <row r="14" spans="2:29">
+      <c r="AB13" s="19"/>
+      <c r="AD13" s="19"/>
+    </row>
+    <row r="14" spans="2:30">
       <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
@@ -2380,19 +2704,19 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
         <v>27</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>6</v>
       </c>
-      <c r="AA14" s="20"/>
-      <c r="AC14" s="20"/>
-    </row>
-    <row r="15" spans="2:29" ht="23.25">
+      <c r="AB14" s="20"/>
+      <c r="AD14" s="20"/>
+    </row>
+    <row r="15" spans="2:30" ht="23.25">
       <c r="B15" s="5" t="s">
         <v>37</v>
       </c>
@@ -2419,19 +2743,19 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>43</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>8</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>362</v>
       </c>
-      <c r="AA15" s="21"/>
-      <c r="AC15" s="21"/>
-    </row>
-    <row r="16" spans="2:29">
+      <c r="AB15" s="21"/>
+      <c r="AD15" s="21"/>
+    </row>
+    <row r="16" spans="2:30">
       <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
@@ -2458,544 +2782,844 @@
       <c r="O16">
         <v>35</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>21</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="16"/>
-      <c r="AC16" s="16"/>
-    </row>
-    <row r="17" spans="27:29" ht="16.5">
-      <c r="AA17" s="17"/>
-      <c r="AC17" s="17"/>
-    </row>
-    <row r="18" spans="27:29" ht="16.5">
-      <c r="AA18" s="22"/>
-      <c r="AC18" s="22"/>
-    </row>
-    <row r="19" spans="27:29" ht="16.5">
-      <c r="AA19" s="23"/>
-      <c r="AC19" s="23"/>
-    </row>
-    <row r="20" spans="27:29" ht="16.5">
-      <c r="AA20" s="22"/>
-      <c r="AC20" s="22"/>
-    </row>
-    <row r="21" spans="27:29" ht="16.5">
-      <c r="AA21" s="17"/>
-      <c r="AC21" s="17"/>
-    </row>
-    <row r="22" spans="27:29" ht="16.5">
-      <c r="AA22" s="24"/>
-      <c r="AC22" s="24"/>
-    </row>
-    <row r="23" spans="27:29" ht="16.5">
-      <c r="AA23" s="23"/>
-      <c r="AC23" s="23"/>
-    </row>
-    <row r="24" spans="27:29" ht="16.5">
-      <c r="AA24" s="24"/>
-      <c r="AC24" s="24"/>
-    </row>
-    <row r="25" spans="27:29" ht="16.5">
-      <c r="AA25" s="25"/>
-      <c r="AC25" s="25"/>
-    </row>
-    <row r="26" spans="27:29" ht="16.5">
-      <c r="AA26" s="24"/>
-      <c r="AC26" s="24"/>
-    </row>
-    <row r="27" spans="27:29" ht="16.5">
-      <c r="AA27" s="23"/>
-      <c r="AC27" s="23"/>
-    </row>
-    <row r="28" spans="27:29" ht="16.5">
-      <c r="AA28" s="24"/>
-      <c r="AC28" s="24"/>
-    </row>
-    <row r="29" spans="27:29" ht="16.5">
-      <c r="AA29" s="25"/>
-      <c r="AC29" s="25"/>
-    </row>
-    <row r="30" spans="27:29" ht="16.5">
-      <c r="AA30" s="24"/>
-      <c r="AC30" s="24"/>
-    </row>
-    <row r="31" spans="27:29" ht="16.5">
-      <c r="AA31" s="23"/>
-      <c r="AC31" s="23"/>
-    </row>
-    <row r="32" spans="27:29" ht="16.5">
-      <c r="AA32" s="24"/>
-      <c r="AC32" s="24"/>
-    </row>
-    <row r="33" spans="27:29" ht="16.5">
-      <c r="AA33" s="25"/>
-      <c r="AC33" s="25"/>
-    </row>
-    <row r="34" spans="27:29" ht="16.5">
-      <c r="AA34" s="24"/>
-      <c r="AC34" s="24"/>
-    </row>
-    <row r="35" spans="27:29" ht="16.5">
-      <c r="AA35" s="26"/>
-      <c r="AC35" s="26"/>
-    </row>
-    <row r="36" spans="27:29" ht="16.5">
-      <c r="AA36" s="24"/>
-      <c r="AC36" s="24"/>
-    </row>
-    <row r="37" spans="27:29" ht="16.5">
-      <c r="AA37" s="25"/>
-      <c r="AC37" s="25"/>
-    </row>
-    <row r="38" spans="27:29" ht="16.5">
-      <c r="AA38" s="24"/>
-      <c r="AC38" s="24"/>
-    </row>
-    <row r="39" spans="27:29" ht="16.5">
-      <c r="AA39" s="26"/>
-      <c r="AC39" s="26"/>
-    </row>
-    <row r="40" spans="27:29" ht="16.5">
-      <c r="AA40" s="24"/>
-      <c r="AC40" s="24"/>
-    </row>
-    <row r="41" spans="27:29" ht="16.5">
-      <c r="AA41" s="25"/>
-      <c r="AC41" s="25"/>
-    </row>
-    <row r="42" spans="27:29" ht="16.5">
-      <c r="AA42" s="24"/>
-      <c r="AC42" s="24"/>
-    </row>
-    <row r="43" spans="27:29" ht="16.5">
-      <c r="AA43" s="26"/>
-      <c r="AC43" s="26"/>
-    </row>
-    <row r="44" spans="27:29" ht="16.5">
-      <c r="AA44" s="24"/>
-      <c r="AC44" s="24"/>
-    </row>
-    <row r="45" spans="27:29" ht="16.5">
-      <c r="AA45" s="25"/>
-      <c r="AC45" s="25"/>
-    </row>
-    <row r="46" spans="27:29" ht="16.5">
-      <c r="AA46" s="24"/>
-      <c r="AC46" s="24"/>
-    </row>
-    <row r="47" spans="27:29" ht="16.5">
-      <c r="AA47" s="26"/>
-      <c r="AC47" s="26"/>
-    </row>
-    <row r="48" spans="27:29" ht="16.5">
-      <c r="AA48" s="24"/>
-      <c r="AC48" s="24"/>
-    </row>
-    <row r="49" spans="27:29" ht="16.5">
-      <c r="AA49" s="25"/>
-      <c r="AC49" s="25"/>
-    </row>
-    <row r="50" spans="27:29" ht="16.5">
-      <c r="AA50" s="24"/>
-      <c r="AC50" s="24"/>
-    </row>
-    <row r="51" spans="27:29" ht="16.5">
-      <c r="AA51" s="26"/>
-      <c r="AC51" s="26"/>
-    </row>
-    <row r="52" spans="27:29" ht="16.5">
-      <c r="AA52" s="24"/>
-      <c r="AC52" s="24"/>
-    </row>
-    <row r="53" spans="27:29" ht="16.5">
-      <c r="AA53" s="25"/>
-      <c r="AC53" s="25"/>
-    </row>
-    <row r="54" spans="27:29" ht="16.5">
-      <c r="AA54" s="24"/>
-      <c r="AC54" s="24"/>
-    </row>
-    <row r="55" spans="27:29" ht="16.5">
-      <c r="AA55" s="26"/>
-      <c r="AC55" s="26"/>
-    </row>
-    <row r="56" spans="27:29" ht="16.5">
-      <c r="AA56" s="24"/>
-      <c r="AC56" s="24"/>
-    </row>
-    <row r="57" spans="27:29" ht="16.5">
-      <c r="AA57" s="25"/>
-      <c r="AC57" s="25"/>
-    </row>
-    <row r="58" spans="27:29" ht="16.5">
-      <c r="AA58" s="24"/>
-      <c r="AC58" s="24"/>
-    </row>
-    <row r="59" spans="27:29" ht="16.5">
-      <c r="AA59" s="26"/>
-      <c r="AC59" s="26"/>
-    </row>
-    <row r="60" spans="27:29" ht="16.5">
-      <c r="AA60" s="24"/>
-      <c r="AC60" s="24"/>
-    </row>
-    <row r="61" spans="27:29" ht="16.5">
-      <c r="AA61" s="25"/>
-      <c r="AC61" s="25"/>
-    </row>
-    <row r="62" spans="27:29" ht="16.5">
-      <c r="AA62" s="24"/>
-      <c r="AC62" s="24"/>
-    </row>
-    <row r="63" spans="27:29" ht="16.5">
-      <c r="AA63" s="26"/>
-      <c r="AC63" s="26"/>
-    </row>
-    <row r="64" spans="27:29" ht="16.5">
-      <c r="AA64" s="24"/>
-      <c r="AC64" s="24"/>
-    </row>
-    <row r="65" spans="27:29" ht="16.5">
-      <c r="AA65" s="25"/>
-      <c r="AC65" s="25"/>
-    </row>
-    <row r="66" spans="27:29" ht="16.5">
-      <c r="AA66" s="24"/>
-      <c r="AC66" s="24"/>
-    </row>
-    <row r="67" spans="27:29" ht="16.5">
-      <c r="AA67" s="26"/>
-      <c r="AC67" s="26"/>
-    </row>
-    <row r="68" spans="27:29" ht="16.5">
-      <c r="AA68" s="24"/>
-      <c r="AC68" s="24"/>
-    </row>
-    <row r="69" spans="27:29" ht="16.5">
-      <c r="AA69" s="25"/>
-      <c r="AC69" s="25"/>
-    </row>
-    <row r="70" spans="27:29" ht="16.5">
-      <c r="AA70" s="24"/>
-      <c r="AC70" s="24"/>
-    </row>
-    <row r="71" spans="27:29" ht="16.5">
-      <c r="AA71" s="26"/>
-      <c r="AC71" s="26"/>
-    </row>
-    <row r="72" spans="27:29" ht="16.5">
-      <c r="AA72" s="24"/>
-      <c r="AC72" s="24"/>
-    </row>
-    <row r="73" spans="27:29" ht="16.5">
-      <c r="AA73" s="25"/>
-      <c r="AC73" s="25"/>
-    </row>
-    <row r="74" spans="27:29" ht="16.5">
-      <c r="AA74" s="24"/>
-      <c r="AC74" s="24"/>
-    </row>
-    <row r="75" spans="27:29" ht="16.5">
-      <c r="AA75" s="26"/>
-      <c r="AC75" s="26"/>
-    </row>
-    <row r="76" spans="27:29" ht="16.5">
-      <c r="AA76" s="24"/>
-      <c r="AC76" s="24"/>
-    </row>
-    <row r="77" spans="27:29" ht="16.5">
-      <c r="AA77" s="25"/>
-      <c r="AC77" s="25"/>
-    </row>
-    <row r="78" spans="27:29" ht="16.5">
-      <c r="AA78" s="24"/>
-      <c r="AC78" s="24"/>
-    </row>
-    <row r="79" spans="27:29" ht="16.5">
-      <c r="AA79" s="26"/>
-      <c r="AC79" s="26"/>
-    </row>
-    <row r="80" spans="27:29" ht="16.5">
-      <c r="AA80" s="24"/>
-      <c r="AC80" s="24"/>
-    </row>
-    <row r="81" spans="27:29" ht="16.5">
-      <c r="AA81" s="25"/>
-      <c r="AC81" s="25"/>
-    </row>
-    <row r="82" spans="27:29" ht="16.5">
-      <c r="AA82" s="24"/>
-      <c r="AC82" s="24"/>
-    </row>
-    <row r="83" spans="27:29" ht="16.5">
-      <c r="AA83" s="26"/>
-      <c r="AC83" s="26"/>
-    </row>
-    <row r="84" spans="27:29" ht="16.5">
-      <c r="AA84" s="24"/>
-      <c r="AC84" s="24"/>
-    </row>
-    <row r="85" spans="27:29" ht="16.5">
-      <c r="AA85" s="25"/>
-      <c r="AC85" s="25"/>
-    </row>
-    <row r="86" spans="27:29" ht="16.5">
-      <c r="AA86" s="24"/>
-      <c r="AC86" s="24"/>
-    </row>
-    <row r="87" spans="27:29" ht="16.5">
-      <c r="AA87" s="26"/>
-      <c r="AC87" s="26"/>
-    </row>
-    <row r="88" spans="27:29" ht="16.5">
-      <c r="AA88" s="24"/>
-      <c r="AC88" s="24"/>
-    </row>
-    <row r="89" spans="27:29" ht="16.5">
-      <c r="AA89" s="25"/>
-      <c r="AC89" s="25"/>
-    </row>
-    <row r="90" spans="27:29" ht="16.5">
-      <c r="AA90" s="24"/>
-      <c r="AC90" s="24"/>
-    </row>
-    <row r="91" spans="27:29" ht="16.5">
-      <c r="AA91" s="26"/>
-      <c r="AC91" s="26"/>
-    </row>
-    <row r="92" spans="27:29" ht="16.5">
-      <c r="AA92" s="24"/>
-      <c r="AC92" s="24"/>
-    </row>
-    <row r="93" spans="27:29" ht="16.5">
-      <c r="AA93" s="25"/>
-      <c r="AC93" s="25"/>
-    </row>
-    <row r="94" spans="27:29" ht="16.5">
-      <c r="AA94" s="24"/>
-      <c r="AC94" s="24"/>
-    </row>
-    <row r="95" spans="27:29" ht="16.5">
-      <c r="AA95" s="26"/>
-      <c r="AC95" s="26"/>
-    </row>
-    <row r="96" spans="27:29" ht="16.5">
-      <c r="AA96" s="24"/>
-      <c r="AC96" s="24"/>
-    </row>
-    <row r="97" spans="27:29" ht="16.5">
-      <c r="AA97" s="25"/>
-      <c r="AC97" s="25"/>
-    </row>
-    <row r="98" spans="27:29" ht="16.5">
-      <c r="AA98" s="24"/>
-      <c r="AC98" s="24"/>
-    </row>
-    <row r="99" spans="27:29" ht="16.5">
-      <c r="AA99" s="26"/>
-      <c r="AC99" s="26"/>
-    </row>
-    <row r="100" spans="27:29" ht="16.5">
-      <c r="AA100" s="24"/>
-      <c r="AC100" s="24"/>
-    </row>
-    <row r="101" spans="27:29" ht="16.5">
-      <c r="AA101" s="25"/>
-      <c r="AC101" s="25"/>
-    </row>
-    <row r="102" spans="27:29" ht="16.5">
-      <c r="AA102" s="24"/>
-      <c r="AC102" s="24"/>
-    </row>
-    <row r="103" spans="27:29" ht="16.5">
-      <c r="AA103" s="26"/>
-      <c r="AC103" s="26"/>
-    </row>
-    <row r="104" spans="27:29" ht="16.5">
-      <c r="AA104" s="24"/>
-      <c r="AC104" s="24"/>
-    </row>
-    <row r="105" spans="27:29" ht="16.5">
-      <c r="AA105" s="25"/>
-      <c r="AC105" s="25"/>
-    </row>
-    <row r="106" spans="27:29" ht="16.5">
-      <c r="AA106" s="24"/>
-      <c r="AC106" s="24"/>
-    </row>
-    <row r="107" spans="27:29" ht="16.5">
-      <c r="AA107" s="26"/>
-      <c r="AC107" s="26"/>
-    </row>
-    <row r="108" spans="27:29" ht="16.5">
-      <c r="AA108" s="24"/>
-      <c r="AC108" s="24"/>
-    </row>
-    <row r="109" spans="27:29" ht="16.5">
-      <c r="AA109" s="25"/>
-      <c r="AC109" s="25"/>
-    </row>
-    <row r="110" spans="27:29" ht="16.5">
-      <c r="AA110" s="24"/>
-      <c r="AC110" s="24"/>
-    </row>
-    <row r="111" spans="27:29" ht="16.5">
-      <c r="AA111" s="26"/>
-      <c r="AC111" s="26"/>
-    </row>
-    <row r="112" spans="27:29" ht="16.5">
-      <c r="AA112" s="24"/>
-      <c r="AC112" s="24"/>
-    </row>
-    <row r="113" spans="27:29" ht="16.5">
-      <c r="AA113" s="25"/>
-      <c r="AC113" s="25"/>
-    </row>
-    <row r="114" spans="27:29" ht="16.5">
-      <c r="AA114" s="24"/>
-      <c r="AC114" s="24"/>
-    </row>
-    <row r="115" spans="27:29" ht="16.5">
-      <c r="AA115" s="26"/>
-      <c r="AC115" s="26"/>
-    </row>
-    <row r="116" spans="27:29" ht="16.5">
-      <c r="AA116" s="24"/>
-      <c r="AC116" s="24"/>
-    </row>
-    <row r="117" spans="27:29" ht="16.5">
-      <c r="AA117" s="25"/>
-      <c r="AC117" s="25"/>
-    </row>
-    <row r="118" spans="27:29" ht="16.5">
-      <c r="AA118" s="24"/>
-      <c r="AC118" s="24"/>
-    </row>
-    <row r="119" spans="27:29" ht="16.5">
-      <c r="AA119" s="26"/>
-      <c r="AC119" s="26"/>
-    </row>
-    <row r="120" spans="27:29" ht="16.5">
-      <c r="AA120" s="24"/>
-      <c r="AC120" s="24"/>
-    </row>
-    <row r="121" spans="27:29" ht="16.5">
-      <c r="AA121" s="25"/>
-      <c r="AC121" s="25"/>
-    </row>
-    <row r="122" spans="27:29" ht="16.5">
-      <c r="AA122" s="24"/>
-      <c r="AC122" s="24"/>
-    </row>
-    <row r="123" spans="27:29" ht="16.5">
-      <c r="AA123" s="26"/>
-      <c r="AC123" s="26"/>
-    </row>
-    <row r="124" spans="27:29" ht="16.5">
-      <c r="AA124" s="24"/>
-      <c r="AC124" s="24"/>
-    </row>
-    <row r="125" spans="27:29" ht="16.5">
-      <c r="AA125" s="25"/>
-      <c r="AC125" s="25"/>
-    </row>
-    <row r="126" spans="27:29" ht="16.5">
-      <c r="AA126" s="24"/>
-      <c r="AC126" s="24"/>
-    </row>
-    <row r="127" spans="27:29" ht="16.5">
-      <c r="AA127" s="26"/>
-      <c r="AC127" s="26"/>
-    </row>
-    <row r="128" spans="27:29" ht="16.5">
-      <c r="AA128" s="24"/>
-      <c r="AC128" s="24"/>
-    </row>
-    <row r="129" spans="27:29" ht="16.5">
-      <c r="AA129" s="25"/>
-      <c r="AC129" s="25"/>
-    </row>
-    <row r="130" spans="27:29" ht="16.5">
-      <c r="AA130" s="24"/>
-      <c r="AC130" s="24"/>
-    </row>
-    <row r="131" spans="27:29" ht="16.5">
-      <c r="AA131" s="26"/>
-      <c r="AC131" s="26"/>
-    </row>
-    <row r="132" spans="27:29" ht="16.5">
-      <c r="AA132" s="24"/>
-      <c r="AC132" s="24"/>
-    </row>
-    <row r="133" spans="27:29" ht="16.5">
-      <c r="AA133" s="25"/>
-      <c r="AC133" s="25"/>
-    </row>
-    <row r="134" spans="27:29" ht="16.5">
-      <c r="AA134" s="24"/>
-      <c r="AC134" s="24"/>
-    </row>
-    <row r="135" spans="27:29" ht="16.5">
-      <c r="AA135" s="26"/>
-      <c r="AC135" s="26"/>
-    </row>
-    <row r="136" spans="27:29" ht="16.5">
-      <c r="AA136" s="24"/>
-      <c r="AC136" s="24"/>
-    </row>
-    <row r="137" spans="27:29" ht="16.5">
-      <c r="AA137" s="25"/>
-      <c r="AC137" s="25"/>
-    </row>
-    <row r="138" spans="27:29" ht="16.5">
-      <c r="AA138" s="24"/>
-      <c r="AC138" s="24"/>
-    </row>
-    <row r="139" spans="27:29" ht="16.5">
-      <c r="AA139" s="26"/>
-      <c r="AC139" s="26"/>
-    </row>
-    <row r="140" spans="27:29" ht="16.5">
-      <c r="AA140" s="24"/>
-      <c r="AC140" s="24"/>
-    </row>
-    <row r="141" spans="27:29" ht="16.5">
-      <c r="AA141" s="25"/>
-      <c r="AC141" s="25"/>
-    </row>
-    <row r="142" spans="27:29" ht="16.5">
-      <c r="AA142" s="24"/>
-      <c r="AC142" s="24"/>
-    </row>
-    <row r="143" spans="27:29" ht="16.5">
-      <c r="AA143" s="26"/>
-      <c r="AC143" s="26"/>
-    </row>
-    <row r="144" spans="27:29" ht="16.5">
-      <c r="AA144" s="24"/>
-      <c r="AC144" s="24"/>
-    </row>
-    <row r="145" spans="27:29" ht="16.5">
-      <c r="AA145" s="25"/>
-      <c r="AC145" s="25"/>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="16"/>
+      <c r="AD16" s="16"/>
+    </row>
+    <row r="17" spans="2:30" ht="16.5">
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44069</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>23</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>14</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="17"/>
+      <c r="AD17" s="17"/>
+    </row>
+    <row r="18" spans="2:30" ht="16.5">
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44069</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>8</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="22"/>
+      <c r="AD18" s="22"/>
+    </row>
+    <row r="19" spans="2:30" ht="16.5">
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44069</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>35</v>
+      </c>
+      <c r="Q19">
+        <v>21</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>13</v>
+      </c>
+      <c r="T19">
+        <v>10</v>
+      </c>
+      <c r="AB19" s="23"/>
+      <c r="AD19" s="23"/>
+    </row>
+    <row r="20" spans="2:30" ht="16.5">
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20">
+        <v>72</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="Q20">
+        <v>37</v>
+      </c>
+      <c r="R20">
+        <v>8</v>
+      </c>
+      <c r="AB20" s="22"/>
+      <c r="AD20" s="22"/>
+    </row>
+    <row r="21" spans="2:30" ht="16.5">
+      <c r="B21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>18</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="17"/>
+      <c r="AD21" s="17"/>
+    </row>
+    <row r="22" spans="2:30" ht="16.5">
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>35</v>
+      </c>
+      <c r="Q22">
+        <v>21</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>13</v>
+      </c>
+      <c r="T22">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="24"/>
+      <c r="AD22" s="24"/>
+    </row>
+    <row r="23" spans="2:30" ht="16.5">
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44083</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="G23">
+        <v>43</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+      <c r="P23">
+        <v>80</v>
+      </c>
+      <c r="Q23">
+        <v>62</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="23"/>
+      <c r="AD23" s="23"/>
+    </row>
+    <row r="24" spans="2:30" ht="16.5">
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44083</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>8</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>8</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="24"/>
+      <c r="AD24" s="24"/>
+    </row>
+    <row r="25" spans="2:30" ht="16.5">
+      <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44083</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>35</v>
+      </c>
+      <c r="Q25">
+        <v>21</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>13</v>
+      </c>
+      <c r="T25">
+        <v>5</v>
+      </c>
+      <c r="AB25" s="25"/>
+      <c r="AD25" s="25"/>
+    </row>
+    <row r="26" spans="2:30" ht="16.5">
+      <c r="AB26" s="24"/>
+      <c r="AD26" s="24"/>
+    </row>
+    <row r="27" spans="2:30" ht="16.5">
+      <c r="AB27" s="23"/>
+      <c r="AD27" s="23"/>
+    </row>
+    <row r="28" spans="2:30" ht="16.5">
+      <c r="AB28" s="24"/>
+      <c r="AD28" s="24"/>
+    </row>
+    <row r="29" spans="2:30" ht="16.5">
+      <c r="AB29" s="25"/>
+      <c r="AD29" s="25"/>
+    </row>
+    <row r="30" spans="2:30" ht="16.5">
+      <c r="AB30" s="24"/>
+      <c r="AD30" s="24"/>
+    </row>
+    <row r="31" spans="2:30" ht="16.5">
+      <c r="AB31" s="23"/>
+      <c r="AD31" s="23"/>
+    </row>
+    <row r="32" spans="2:30" ht="16.5">
+      <c r="AB32" s="24"/>
+      <c r="AD32" s="24"/>
+    </row>
+    <row r="33" spans="28:30" ht="16.5">
+      <c r="AB33" s="25"/>
+      <c r="AD33" s="25"/>
+    </row>
+    <row r="34" spans="28:30" ht="16.5">
+      <c r="AB34" s="24"/>
+      <c r="AD34" s="24"/>
+    </row>
+    <row r="35" spans="28:30" ht="16.5">
+      <c r="AB35" s="26"/>
+      <c r="AD35" s="26"/>
+    </row>
+    <row r="36" spans="28:30" ht="16.5">
+      <c r="AB36" s="24"/>
+      <c r="AD36" s="24"/>
+    </row>
+    <row r="37" spans="28:30" ht="16.5">
+      <c r="AB37" s="25"/>
+      <c r="AD37" s="25"/>
+    </row>
+    <row r="38" spans="28:30" ht="16.5">
+      <c r="AB38" s="24"/>
+      <c r="AD38" s="24"/>
+    </row>
+    <row r="39" spans="28:30" ht="16.5">
+      <c r="AB39" s="26"/>
+      <c r="AD39" s="26"/>
+    </row>
+    <row r="40" spans="28:30" ht="16.5">
+      <c r="AB40" s="24"/>
+      <c r="AD40" s="24"/>
+    </row>
+    <row r="41" spans="28:30" ht="16.5">
+      <c r="AB41" s="25"/>
+      <c r="AD41" s="25"/>
+    </row>
+    <row r="42" spans="28:30" ht="16.5">
+      <c r="AB42" s="24"/>
+      <c r="AD42" s="24"/>
+    </row>
+    <row r="43" spans="28:30" ht="16.5">
+      <c r="AB43" s="26"/>
+      <c r="AD43" s="26"/>
+    </row>
+    <row r="44" spans="28:30" ht="16.5">
+      <c r="AB44" s="24"/>
+      <c r="AD44" s="24"/>
+    </row>
+    <row r="45" spans="28:30" ht="16.5">
+      <c r="AB45" s="25"/>
+      <c r="AD45" s="25"/>
+    </row>
+    <row r="46" spans="28:30" ht="16.5">
+      <c r="AB46" s="24"/>
+      <c r="AD46" s="24"/>
+    </row>
+    <row r="47" spans="28:30" ht="16.5">
+      <c r="AB47" s="26"/>
+      <c r="AD47" s="26"/>
+    </row>
+    <row r="48" spans="28:30" ht="16.5">
+      <c r="AB48" s="24"/>
+      <c r="AD48" s="24"/>
+    </row>
+    <row r="49" spans="28:30" ht="16.5">
+      <c r="AB49" s="25"/>
+      <c r="AD49" s="25"/>
+    </row>
+    <row r="50" spans="28:30" ht="16.5">
+      <c r="AB50" s="24"/>
+      <c r="AD50" s="24"/>
+    </row>
+    <row r="51" spans="28:30" ht="16.5">
+      <c r="AB51" s="26"/>
+      <c r="AD51" s="26"/>
+    </row>
+    <row r="52" spans="28:30" ht="16.5">
+      <c r="AB52" s="24"/>
+      <c r="AD52" s="24"/>
+    </row>
+    <row r="53" spans="28:30" ht="16.5">
+      <c r="AB53" s="25"/>
+      <c r="AD53" s="25"/>
+    </row>
+    <row r="54" spans="28:30" ht="16.5">
+      <c r="AB54" s="24"/>
+      <c r="AD54" s="24"/>
+    </row>
+    <row r="55" spans="28:30" ht="16.5">
+      <c r="AB55" s="26"/>
+      <c r="AD55" s="26"/>
+    </row>
+    <row r="56" spans="28:30" ht="16.5">
+      <c r="AB56" s="24"/>
+      <c r="AD56" s="24"/>
+    </row>
+    <row r="57" spans="28:30" ht="16.5">
+      <c r="AB57" s="25"/>
+      <c r="AD57" s="25"/>
+    </row>
+    <row r="58" spans="28:30" ht="16.5">
+      <c r="AB58" s="24"/>
+      <c r="AD58" s="24"/>
+    </row>
+    <row r="59" spans="28:30" ht="16.5">
+      <c r="AB59" s="26"/>
+      <c r="AD59" s="26"/>
+    </row>
+    <row r="60" spans="28:30" ht="16.5">
+      <c r="AB60" s="24"/>
+      <c r="AD60" s="24"/>
+    </row>
+    <row r="61" spans="28:30" ht="16.5">
+      <c r="AB61" s="25"/>
+      <c r="AD61" s="25"/>
+    </row>
+    <row r="62" spans="28:30" ht="16.5">
+      <c r="AB62" s="24"/>
+      <c r="AD62" s="24"/>
+    </row>
+    <row r="63" spans="28:30" ht="16.5">
+      <c r="AB63" s="26"/>
+      <c r="AD63" s="26"/>
+    </row>
+    <row r="64" spans="28:30" ht="16.5">
+      <c r="AB64" s="24"/>
+      <c r="AD64" s="24"/>
+    </row>
+    <row r="65" spans="28:30" ht="16.5">
+      <c r="AB65" s="25"/>
+      <c r="AD65" s="25"/>
+    </row>
+    <row r="66" spans="28:30" ht="16.5">
+      <c r="AB66" s="24"/>
+      <c r="AD66" s="24"/>
+    </row>
+    <row r="67" spans="28:30" ht="16.5">
+      <c r="AB67" s="26"/>
+      <c r="AD67" s="26"/>
+    </row>
+    <row r="68" spans="28:30" ht="16.5">
+      <c r="AB68" s="24"/>
+      <c r="AD68" s="24"/>
+    </row>
+    <row r="69" spans="28:30" ht="16.5">
+      <c r="AB69" s="25"/>
+      <c r="AD69" s="25"/>
+    </row>
+    <row r="70" spans="28:30" ht="16.5">
+      <c r="AB70" s="24"/>
+      <c r="AD70" s="24"/>
+    </row>
+    <row r="71" spans="28:30" ht="16.5">
+      <c r="AB71" s="26"/>
+      <c r="AD71" s="26"/>
+    </row>
+    <row r="72" spans="28:30" ht="16.5">
+      <c r="AB72" s="24"/>
+      <c r="AD72" s="24"/>
+    </row>
+    <row r="73" spans="28:30" ht="16.5">
+      <c r="AB73" s="25"/>
+      <c r="AD73" s="25"/>
+    </row>
+    <row r="74" spans="28:30" ht="16.5">
+      <c r="AB74" s="24"/>
+      <c r="AD74" s="24"/>
+    </row>
+    <row r="75" spans="28:30" ht="16.5">
+      <c r="AB75" s="26"/>
+      <c r="AD75" s="26"/>
+    </row>
+    <row r="76" spans="28:30" ht="16.5">
+      <c r="AB76" s="24"/>
+      <c r="AD76" s="24"/>
+    </row>
+    <row r="77" spans="28:30" ht="16.5">
+      <c r="AB77" s="25"/>
+      <c r="AD77" s="25"/>
+    </row>
+    <row r="78" spans="28:30" ht="16.5">
+      <c r="AB78" s="24"/>
+      <c r="AD78" s="24"/>
+    </row>
+    <row r="79" spans="28:30" ht="16.5">
+      <c r="AB79" s="26"/>
+      <c r="AD79" s="26"/>
+    </row>
+    <row r="80" spans="28:30" ht="16.5">
+      <c r="AB80" s="24"/>
+      <c r="AD80" s="24"/>
+    </row>
+    <row r="81" spans="28:30" ht="16.5">
+      <c r="AB81" s="25"/>
+      <c r="AD81" s="25"/>
+    </row>
+    <row r="82" spans="28:30" ht="16.5">
+      <c r="AB82" s="24"/>
+      <c r="AD82" s="24"/>
+    </row>
+    <row r="83" spans="28:30" ht="16.5">
+      <c r="AB83" s="26"/>
+      <c r="AD83" s="26"/>
+    </row>
+    <row r="84" spans="28:30" ht="16.5">
+      <c r="AB84" s="24"/>
+      <c r="AD84" s="24"/>
+    </row>
+    <row r="85" spans="28:30" ht="16.5">
+      <c r="AB85" s="25"/>
+      <c r="AD85" s="25"/>
+    </row>
+    <row r="86" spans="28:30" ht="16.5">
+      <c r="AB86" s="24"/>
+      <c r="AD86" s="24"/>
+    </row>
+    <row r="87" spans="28:30" ht="16.5">
+      <c r="AB87" s="26"/>
+      <c r="AD87" s="26"/>
+    </row>
+    <row r="88" spans="28:30" ht="16.5">
+      <c r="AB88" s="24"/>
+      <c r="AD88" s="24"/>
+    </row>
+    <row r="89" spans="28:30" ht="16.5">
+      <c r="AB89" s="25"/>
+      <c r="AD89" s="25"/>
+    </row>
+    <row r="90" spans="28:30" ht="16.5">
+      <c r="AB90" s="24"/>
+      <c r="AD90" s="24"/>
+    </row>
+    <row r="91" spans="28:30" ht="16.5">
+      <c r="AB91" s="26"/>
+      <c r="AD91" s="26"/>
+    </row>
+    <row r="92" spans="28:30" ht="16.5">
+      <c r="AB92" s="24"/>
+      <c r="AD92" s="24"/>
+    </row>
+    <row r="93" spans="28:30" ht="16.5">
+      <c r="AB93" s="25"/>
+      <c r="AD93" s="25"/>
+    </row>
+    <row r="94" spans="28:30" ht="16.5">
+      <c r="AB94" s="24"/>
+      <c r="AD94" s="24"/>
+    </row>
+    <row r="95" spans="28:30" ht="16.5">
+      <c r="AB95" s="26"/>
+      <c r="AD95" s="26"/>
+    </row>
+    <row r="96" spans="28:30" ht="16.5">
+      <c r="AB96" s="24"/>
+      <c r="AD96" s="24"/>
+    </row>
+    <row r="97" spans="28:30" ht="16.5">
+      <c r="AB97" s="25"/>
+      <c r="AD97" s="25"/>
+    </row>
+    <row r="98" spans="28:30" ht="16.5">
+      <c r="AB98" s="24"/>
+      <c r="AD98" s="24"/>
+    </row>
+    <row r="99" spans="28:30" ht="16.5">
+      <c r="AB99" s="26"/>
+      <c r="AD99" s="26"/>
+    </row>
+    <row r="100" spans="28:30" ht="16.5">
+      <c r="AB100" s="24"/>
+      <c r="AD100" s="24"/>
+    </row>
+    <row r="101" spans="28:30" ht="16.5">
+      <c r="AB101" s="25"/>
+      <c r="AD101" s="25"/>
+    </row>
+    <row r="102" spans="28:30" ht="16.5">
+      <c r="AB102" s="24"/>
+      <c r="AD102" s="24"/>
+    </row>
+    <row r="103" spans="28:30" ht="16.5">
+      <c r="AB103" s="26"/>
+      <c r="AD103" s="26"/>
+    </row>
+    <row r="104" spans="28:30" ht="16.5">
+      <c r="AB104" s="24"/>
+      <c r="AD104" s="24"/>
+    </row>
+    <row r="105" spans="28:30" ht="16.5">
+      <c r="AB105" s="25"/>
+      <c r="AD105" s="25"/>
+    </row>
+    <row r="106" spans="28:30" ht="16.5">
+      <c r="AB106" s="24"/>
+      <c r="AD106" s="24"/>
+    </row>
+    <row r="107" spans="28:30" ht="16.5">
+      <c r="AB107" s="26"/>
+      <c r="AD107" s="26"/>
+    </row>
+    <row r="108" spans="28:30" ht="16.5">
+      <c r="AB108" s="24"/>
+      <c r="AD108" s="24"/>
+    </row>
+    <row r="109" spans="28:30" ht="16.5">
+      <c r="AB109" s="25"/>
+      <c r="AD109" s="25"/>
+    </row>
+    <row r="110" spans="28:30" ht="16.5">
+      <c r="AB110" s="24"/>
+      <c r="AD110" s="24"/>
+    </row>
+    <row r="111" spans="28:30" ht="16.5">
+      <c r="AB111" s="26"/>
+      <c r="AD111" s="26"/>
+    </row>
+    <row r="112" spans="28:30" ht="16.5">
+      <c r="AB112" s="24"/>
+      <c r="AD112" s="24"/>
+    </row>
+    <row r="113" spans="28:30" ht="16.5">
+      <c r="AB113" s="25"/>
+      <c r="AD113" s="25"/>
+    </row>
+    <row r="114" spans="28:30" ht="16.5">
+      <c r="AB114" s="24"/>
+      <c r="AD114" s="24"/>
+    </row>
+    <row r="115" spans="28:30" ht="16.5">
+      <c r="AB115" s="26"/>
+      <c r="AD115" s="26"/>
+    </row>
+    <row r="116" spans="28:30" ht="16.5">
+      <c r="AB116" s="24"/>
+      <c r="AD116" s="24"/>
+    </row>
+    <row r="117" spans="28:30" ht="16.5">
+      <c r="AB117" s="25"/>
+      <c r="AD117" s="25"/>
+    </row>
+    <row r="118" spans="28:30" ht="16.5">
+      <c r="AB118" s="24"/>
+      <c r="AD118" s="24"/>
+    </row>
+    <row r="119" spans="28:30" ht="16.5">
+      <c r="AB119" s="26"/>
+      <c r="AD119" s="26"/>
+    </row>
+    <row r="120" spans="28:30" ht="16.5">
+      <c r="AB120" s="24"/>
+      <c r="AD120" s="24"/>
+    </row>
+    <row r="121" spans="28:30" ht="16.5">
+      <c r="AB121" s="25"/>
+      <c r="AD121" s="25"/>
+    </row>
+    <row r="122" spans="28:30" ht="16.5">
+      <c r="AB122" s="24"/>
+      <c r="AD122" s="24"/>
+    </row>
+    <row r="123" spans="28:30" ht="16.5">
+      <c r="AB123" s="26"/>
+      <c r="AD123" s="26"/>
+    </row>
+    <row r="124" spans="28:30" ht="16.5">
+      <c r="AB124" s="24"/>
+      <c r="AD124" s="24"/>
+    </row>
+    <row r="125" spans="28:30" ht="16.5">
+      <c r="AB125" s="25"/>
+      <c r="AD125" s="25"/>
+    </row>
+    <row r="126" spans="28:30" ht="16.5">
+      <c r="AB126" s="24"/>
+      <c r="AD126" s="24"/>
+    </row>
+    <row r="127" spans="28:30" ht="16.5">
+      <c r="AB127" s="26"/>
+      <c r="AD127" s="26"/>
+    </row>
+    <row r="128" spans="28:30" ht="16.5">
+      <c r="AB128" s="24"/>
+      <c r="AD128" s="24"/>
+    </row>
+    <row r="129" spans="28:30" ht="16.5">
+      <c r="AB129" s="25"/>
+      <c r="AD129" s="25"/>
+    </row>
+    <row r="130" spans="28:30" ht="16.5">
+      <c r="AB130" s="24"/>
+      <c r="AD130" s="24"/>
+    </row>
+    <row r="131" spans="28:30" ht="16.5">
+      <c r="AB131" s="26"/>
+      <c r="AD131" s="26"/>
+    </row>
+    <row r="132" spans="28:30" ht="16.5">
+      <c r="AB132" s="24"/>
+      <c r="AD132" s="24"/>
+    </row>
+    <row r="133" spans="28:30" ht="16.5">
+      <c r="AB133" s="25"/>
+      <c r="AD133" s="25"/>
+    </row>
+    <row r="134" spans="28:30" ht="16.5">
+      <c r="AB134" s="24"/>
+      <c r="AD134" s="24"/>
+    </row>
+    <row r="135" spans="28:30" ht="16.5">
+      <c r="AB135" s="26"/>
+      <c r="AD135" s="26"/>
+    </row>
+    <row r="136" spans="28:30" ht="16.5">
+      <c r="AB136" s="24"/>
+      <c r="AD136" s="24"/>
+    </row>
+    <row r="137" spans="28:30" ht="16.5">
+      <c r="AB137" s="25"/>
+      <c r="AD137" s="25"/>
+    </row>
+    <row r="138" spans="28:30" ht="16.5">
+      <c r="AB138" s="24"/>
+      <c r="AD138" s="24"/>
+    </row>
+    <row r="139" spans="28:30" ht="16.5">
+      <c r="AB139" s="26"/>
+      <c r="AD139" s="26"/>
+    </row>
+    <row r="140" spans="28:30" ht="16.5">
+      <c r="AB140" s="24"/>
+      <c r="AD140" s="24"/>
+    </row>
+    <row r="141" spans="28:30" ht="16.5">
+      <c r="AB141" s="25"/>
+      <c r="AD141" s="25"/>
+    </row>
+    <row r="142" spans="28:30" ht="16.5">
+      <c r="AB142" s="24"/>
+      <c r="AD142" s="24"/>
+    </row>
+    <row r="143" spans="28:30" ht="16.5">
+      <c r="AB143" s="26"/>
+      <c r="AD143" s="26"/>
+    </row>
+    <row r="144" spans="28:30" ht="16.5">
+      <c r="AB144" s="24"/>
+      <c r="AD144" s="24"/>
+    </row>
+    <row r="145" spans="28:30" ht="16.5">
+      <c r="AB145" s="25"/>
+      <c r="AD145" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D2:F3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="U2:V3"/>
+    <mergeCell ref="T2:U3"/>
+    <mergeCell ref="V2:W3"/>
     <mergeCell ref="G2:H3"/>
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:M3"/>
-    <mergeCell ref="P2:R3"/>
+    <mergeCell ref="Q2:S3"/>
+    <mergeCell ref="N2:P3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>